<commit_message>
Updates from IW testing
</commit_message>
<xml_diff>
--- a/Ian/siman testing log.xlsx
+++ b/Ian/siman testing log.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\siman\Ian\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\simansuite\Ian\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3E3542E-CA34-44BB-8DBB-03D070997151}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B5324FE-C07A-4B07-9766-B5236A59DD5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$I$68</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$I$67</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="161">
   <si>
     <t>area</t>
   </si>
@@ -518,12 +518,6 @@
   </si>
   <si>
     <t>re-order performance measures in helpfile</t>
-  </si>
-  <si>
-    <t>siman lollyplot</t>
-  </si>
-  <si>
-    <t>by(target) not working</t>
   </si>
   <si>
     <t>doesn’t show graphs split out by dgm if dgm is in the format dgm(dgm1 dgm2 dgm3).  Isn't this format only applicable for nestloop and trellis?  If not, all these other graphs need a separate treatment of dgm if dgm(dgm1 dgm2 dgm3)</t>
@@ -558,18 +552,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -584,7 +572,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -594,12 +582,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -622,11 +604,22 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="8">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
@@ -1006,13 +999,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:J107"/>
+  <dimension ref="A1:J106"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F59" sqref="F59"/>
+      <selection pane="bottomRight" activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1067,192 +1060,192 @@
         <v>152</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="6" customFormat="1" ht="116" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="6">
+    <row r="3" spans="1:10" s="4" customFormat="1" ht="116" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="4">
         <v>1</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="6">
         <v>44684</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="6">
         <v>44742</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="4" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="6" customFormat="1" ht="29" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="6">
+    <row r="4" spans="1:10" s="4" customFormat="1" ht="29" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="4">
         <v>2</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="6">
         <v>44684</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="6">
         <v>44742</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="H4" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="I4" s="4" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="6" customFormat="1" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="6">
+    <row r="5" spans="1:10" s="4" customFormat="1" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="4">
         <v>3</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="6">
         <v>44684</v>
       </c>
-      <c r="F5" s="7"/>
-      <c r="G5" s="8">
+      <c r="F5" s="5"/>
+      <c r="G5" s="6">
         <v>44686</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="H5" s="5" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="6" customFormat="1" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="6">
+    <row r="6" spans="1:10" s="4" customFormat="1" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="4">
         <v>4</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="6">
         <v>44684</v>
       </c>
-      <c r="F6" s="7"/>
-      <c r="G6" s="8">
+      <c r="F6" s="5"/>
+      <c r="G6" s="6">
         <v>44685</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="H6" s="5" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="6" customFormat="1" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="6">
+    <row r="7" spans="1:10" s="4" customFormat="1" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="4">
         <v>5</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="6">
         <v>44684</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="G7" s="8"/>
-      <c r="H7" s="7" t="s">
+      <c r="G7" s="6"/>
+      <c r="H7" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="I7" s="6" t="s">
+      <c r="I7" s="4" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="6" customFormat="1" ht="87" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="6">
+    <row r="8" spans="1:10" s="4" customFormat="1" ht="87" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="4">
         <v>6</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="6">
         <v>44684</v>
       </c>
-      <c r="F8" s="7"/>
-      <c r="G8" s="8">
+      <c r="F8" s="5"/>
+      <c r="G8" s="6">
         <v>44686</v>
       </c>
-      <c r="H8" s="7" t="s">
+      <c r="H8" s="5" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="6" customFormat="1" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="6">
+    <row r="9" spans="1:10" s="4" customFormat="1" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="4">
         <v>7</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="E9" s="11">
+      <c r="E9" s="9">
         <v>44684</v>
       </c>
-      <c r="F9" s="9"/>
-      <c r="G9" s="11">
+      <c r="F9" s="7"/>
+      <c r="G9" s="9">
         <v>44679</v>
       </c>
-      <c r="H9" s="9" t="s">
+      <c r="H9" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="I9" s="6" t="s">
+      <c r="I9" s="4" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="6">
+      <c r="A10" s="4">
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -1275,7 +1268,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="48" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="6">
+      <c r="A11" s="4">
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -1298,10 +1291,10 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="87" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="12">
+      <c r="A12" s="10">
         <v>10</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="8" t="s">
         <v>42</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -1313,13 +1306,13 @@
       <c r="E12" s="2">
         <v>44609</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="F12" s="8" t="s">
         <v>45</v>
       </c>
       <c r="G12" s="2">
         <v>44742</v>
       </c>
-      <c r="H12" s="10" t="s">
+      <c r="H12" s="8" t="s">
         <v>79</v>
       </c>
       <c r="I12" s="1" t="s">
@@ -1327,7 +1320,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="6">
+      <c r="A13" s="4">
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -1349,38 +1342,40 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="6">
+    <row r="14" spans="1:10" s="8" customFormat="1" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="10">
         <v>12</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14" s="5">
-        <v>44609</v>
-      </c>
-      <c r="F14" s="4" t="s">
+      <c r="D14" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="11">
+        <v>44609</v>
+      </c>
+      <c r="F14" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4" t="s">
+      <c r="G14" s="11">
+        <v>44809</v>
+      </c>
+      <c r="H14" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="I14" s="1" t="s">
+      <c r="I14" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="J14" s="1" t="s">
+      <c r="J14" s="8" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="6">
+      <c r="A15" s="4">
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -1403,7 +1398,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" ht="58" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="6">
+      <c r="A16" s="4">
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -1432,7 +1427,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="6">
+      <c r="A17" s="4">
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -1449,7 +1444,7 @@
       </c>
     </row>
     <row r="18" spans="1:9" ht="159.5" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="6">
+      <c r="A18" s="4">
         <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -1469,7 +1464,7 @@
       </c>
     </row>
     <row r="19" spans="1:9" ht="58" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="6">
+      <c r="A19" s="4">
         <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -1486,7 +1481,7 @@
       </c>
     </row>
     <row r="20" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="6">
+      <c r="A20" s="4">
         <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -1509,7 +1504,7 @@
       </c>
     </row>
     <row r="21" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="6">
+      <c r="A21" s="4">
         <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -1529,7 +1524,7 @@
       </c>
     </row>
     <row r="22" spans="1:9" ht="58" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="6">
+      <c r="A22" s="4">
         <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -1552,7 +1547,7 @@
       </c>
     </row>
     <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="6">
+      <c r="A23" s="4">
         <v>21</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -1575,7 +1570,7 @@
       </c>
     </row>
     <row r="24" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="6">
+      <c r="A24" s="4">
         <v>22</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -1598,7 +1593,7 @@
       </c>
     </row>
     <row r="25" spans="1:9" ht="51.65" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="6">
+      <c r="A25" s="4">
         <v>23</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -1618,7 +1613,7 @@
       </c>
     </row>
     <row r="26" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="6">
+      <c r="A26" s="4">
         <v>24</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -1641,7 +1636,7 @@
       </c>
     </row>
     <row r="27" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="6">
+      <c r="A27" s="4">
         <v>25</v>
       </c>
       <c r="B27" s="1" t="s">
@@ -1661,7 +1656,7 @@
       </c>
     </row>
     <row r="28" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="6">
+      <c r="A28" s="4">
         <v>26</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -1684,7 +1679,7 @@
       </c>
     </row>
     <row r="29" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="6">
+      <c r="A29" s="4">
         <v>27</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -1707,7 +1702,7 @@
       </c>
     </row>
     <row r="30" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="6">
+      <c r="A30" s="4">
         <v>28</v>
       </c>
       <c r="B30" s="1" t="s">
@@ -1722,11 +1717,11 @@
       <c r="E30" s="2">
         <v>44609</v>
       </c>
-      <c r="F30" s="10"/>
+      <c r="F30" s="8"/>
       <c r="G30" s="2">
         <v>44742</v>
       </c>
-      <c r="H30" s="10" t="s">
+      <c r="H30" s="8" t="s">
         <v>141</v>
       </c>
       <c r="I30" s="1" t="s">
@@ -1734,7 +1729,7 @@
       </c>
     </row>
     <row r="31" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="6">
+      <c r="A31" s="4">
         <v>29</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -1760,7 +1755,7 @@
       </c>
     </row>
     <row r="32" spans="1:9" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="6">
+      <c r="A32" s="4">
         <v>30</v>
       </c>
       <c r="B32" s="1" t="s">
@@ -1786,7 +1781,7 @@
       </c>
     </row>
     <row r="33" spans="1:9" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="6">
+      <c r="A33" s="4">
         <v>31</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -1804,13 +1799,13 @@
       <c r="G33" s="2">
         <v>44742</v>
       </c>
-      <c r="H33" s="10"/>
+      <c r="H33" s="8"/>
       <c r="I33" s="1" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="6">
+      <c r="A34" s="4">
         <v>32</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -1828,13 +1823,13 @@
       <c r="G34" s="2">
         <v>44742</v>
       </c>
-      <c r="H34" s="10"/>
+      <c r="H34" s="8"/>
       <c r="I34" s="1" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="6">
+      <c r="A35" s="4">
         <v>33</v>
       </c>
       <c r="B35" s="1" t="s">
@@ -1852,12 +1847,12 @@
       <c r="G35" s="2">
         <v>44749</v>
       </c>
-      <c r="H35" s="10" t="s">
+      <c r="H35" s="8" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="6">
+      <c r="A36" s="4">
         <v>34</v>
       </c>
       <c r="B36" s="1" t="s">
@@ -1875,7 +1870,7 @@
       <c r="G36" s="2">
         <v>44742</v>
       </c>
-      <c r="H36" s="10" t="s">
+      <c r="H36" s="8" t="s">
         <v>140</v>
       </c>
       <c r="I36" s="1" t="s">
@@ -1883,7 +1878,7 @@
       </c>
     </row>
     <row r="37" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="6">
+      <c r="A37" s="4">
         <v>35</v>
       </c>
       <c r="B37" s="1" t="s">
@@ -1906,7 +1901,7 @@
       </c>
     </row>
     <row r="38" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="6">
+      <c r="A38" s="4">
         <v>36</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -1926,7 +1921,7 @@
       </c>
     </row>
     <row r="39" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="6">
+      <c r="A39" s="4">
         <v>37</v>
       </c>
       <c r="B39" s="1" t="s">
@@ -1949,7 +1944,7 @@
       </c>
     </row>
     <row r="40" spans="1:9" ht="145" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="6">
+      <c r="A40" s="4">
         <v>38</v>
       </c>
       <c r="B40" s="1" t="s">
@@ -1967,7 +1962,7 @@
       <c r="G40" s="2">
         <v>44742</v>
       </c>
-      <c r="H40" s="10" t="s">
+      <c r="H40" s="8" t="s">
         <v>139</v>
       </c>
       <c r="I40" s="1" t="s">
@@ -1975,7 +1970,7 @@
       </c>
     </row>
     <row r="41" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="6">
+      <c r="A41" s="4">
         <v>39</v>
       </c>
       <c r="B41" s="1" t="s">
@@ -1995,7 +1990,7 @@
       </c>
     </row>
     <row r="42" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="6">
+      <c r="A42" s="4">
         <v>40</v>
       </c>
       <c r="B42" s="1" t="s">
@@ -2015,7 +2010,7 @@
       </c>
     </row>
     <row r="43" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="6">
+      <c r="A43" s="4">
         <v>41</v>
       </c>
       <c r="B43" s="1" t="s">
@@ -2035,7 +2030,7 @@
       </c>
     </row>
     <row r="44" spans="1:9" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="6">
+      <c r="A44" s="4">
         <v>42</v>
       </c>
       <c r="B44" s="1" t="s">
@@ -2055,7 +2050,7 @@
       </c>
     </row>
     <row r="45" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="6">
+      <c r="A45" s="4">
         <v>43</v>
       </c>
       <c r="B45" s="1" t="s">
@@ -2075,7 +2070,7 @@
       </c>
     </row>
     <row r="46" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="6">
+      <c r="A46" s="4">
         <v>44</v>
       </c>
       <c r="B46" s="1" t="s">
@@ -2095,7 +2090,7 @@
       </c>
     </row>
     <row r="47" spans="1:9" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="6">
+      <c r="A47" s="4">
         <v>45</v>
       </c>
       <c r="B47" s="1" t="s">
@@ -2115,7 +2110,7 @@
       </c>
     </row>
     <row r="48" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="6">
+      <c r="A48" s="4">
         <v>46</v>
       </c>
       <c r="B48" s="1" t="s">
@@ -2135,7 +2130,7 @@
       </c>
     </row>
     <row r="49" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="6">
+      <c r="A49" s="4">
         <v>47</v>
       </c>
       <c r="B49" s="1" t="s">
@@ -2155,7 +2150,7 @@
       </c>
     </row>
     <row r="50" spans="1:10" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="6">
+      <c r="A50" s="4">
         <v>48</v>
       </c>
       <c r="B50" s="1" t="s">
@@ -2178,7 +2173,7 @@
       </c>
     </row>
     <row r="51" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="6">
+      <c r="A51" s="4">
         <v>49</v>
       </c>
       <c r="B51" s="1" t="s">
@@ -2198,7 +2193,7 @@
       </c>
     </row>
     <row r="52" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="6">
+      <c r="A52" s="4">
         <v>50</v>
       </c>
       <c r="B52" s="1" t="s">
@@ -2218,7 +2213,7 @@
       </c>
     </row>
     <row r="53" spans="1:10" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="6">
+      <c r="A53" s="4">
         <v>51</v>
       </c>
       <c r="B53" s="1" t="s">
@@ -2238,7 +2233,7 @@
       </c>
     </row>
     <row r="54" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="6">
+      <c r="A54" s="4">
         <v>52</v>
       </c>
       <c r="B54" s="1" t="s">
@@ -2258,7 +2253,7 @@
       </c>
     </row>
     <row r="55" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="6">
+      <c r="A55" s="4">
         <v>53</v>
       </c>
       <c r="B55" s="1" t="s">
@@ -2278,7 +2273,7 @@
       </c>
     </row>
     <row r="56" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="6">
+      <c r="A56" s="4">
         <v>54</v>
       </c>
       <c r="B56" s="1" t="s">
@@ -2298,7 +2293,7 @@
       </c>
     </row>
     <row r="57" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="6">
+      <c r="A57" s="4">
         <v>55</v>
       </c>
       <c r="B57" s="1" t="s">
@@ -2315,7 +2310,7 @@
       </c>
     </row>
     <row r="58" spans="1:10" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="6">
+      <c r="A58" s="4">
         <v>56</v>
       </c>
       <c r="B58" s="1" t="s">
@@ -2332,14 +2327,14 @@
       </c>
     </row>
     <row r="59" spans="1:10" ht="87" x14ac:dyDescent="0.35">
-      <c r="A59" s="6">
+      <c r="A59" s="4">
         <v>57</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>99</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>66</v>
@@ -2350,7 +2345,7 @@
       <c r="F59" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I59" s="6" t="s">
+      <c r="I59" s="4" t="s">
         <v>155</v>
       </c>
       <c r="J59" s="1" t="s">
@@ -2358,7 +2353,7 @@
       </c>
     </row>
     <row r="60" spans="1:10" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="6">
+      <c r="A60" s="4">
         <v>58</v>
       </c>
       <c r="B60" s="1" t="s">
@@ -2375,7 +2370,7 @@
       </c>
     </row>
     <row r="61" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="6">
+      <c r="A61" s="4">
         <v>59</v>
       </c>
       <c r="B61" s="1" t="s">
@@ -2392,7 +2387,7 @@
       </c>
     </row>
     <row r="62" spans="1:10" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="6">
+      <c r="A62" s="4">
         <v>60</v>
       </c>
       <c r="B62" s="1" t="s">
@@ -2412,7 +2407,7 @@
       </c>
     </row>
     <row r="63" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="6">
+      <c r="A63" s="4">
         <v>61</v>
       </c>
       <c r="B63" s="1" t="s">
@@ -2432,7 +2427,7 @@
       </c>
     </row>
     <row r="64" spans="1:10" ht="130.5" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="6">
+      <c r="A64" s="4">
         <v>62</v>
       </c>
       <c r="B64" s="1" t="s">
@@ -2449,7 +2444,7 @@
       </c>
     </row>
     <row r="65" spans="1:10" ht="130.5" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="6">
+      <c r="A65" s="4">
         <v>63</v>
       </c>
       <c r="B65" s="1" t="s">
@@ -2524,21 +2519,7 @@
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A68" s="1">
-        <v>66</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E68" s="2">
-        <v>44802</v>
-      </c>
+      <c r="E68" s="2"/>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.35">
       <c r="E69" s="2"/>
@@ -2654,11 +2635,8 @@
     <row r="106" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E106" s="2"/>
     </row>
-    <row r="107" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E107" s="2"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A2:I68" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <autoFilter ref="A2:I67" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <filterColumn colId="1">
       <filters>
         <filter val="all graphs except nestloop and trellis"/>
@@ -2667,36 +2645,39 @@
       </filters>
     </filterColumn>
     <filterColumn colId="2">
-      <colorFilter dxfId="6" cellColor="0"/>
+      <colorFilter dxfId="7" cellColor="0"/>
+    </filterColumn>
+    <filterColumn colId="5">
+      <colorFilter dxfId="0" cellColor="0"/>
     </filterColumn>
   </autoFilter>
   <conditionalFormatting sqref="A3:G1048576">
-    <cfRule type="expression" dxfId="5" priority="7">
+    <cfRule type="expression" dxfId="6" priority="7">
       <formula>ISBLANK($G3)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10:G10">
-    <cfRule type="expression" dxfId="4" priority="6">
+    <cfRule type="expression" dxfId="5" priority="6">
       <formula>ISBLANK($G10)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11:B13">
-    <cfRule type="expression" dxfId="3" priority="5">
+    <cfRule type="expression" dxfId="4" priority="5">
       <formula>ISBLANK($G11)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11:G13">
-    <cfRule type="expression" dxfId="2" priority="4">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>ISBLANK($G11)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17:G17">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula>ISBLANK($G17)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D18:E20">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>ISBLANK($G18)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>